<commit_message>
style khi insert row
</commit_message>
<xml_diff>
--- a/Worksheet/Content/Template/Default.xlsx
+++ b/Worksheet/Content/Template/Default.xlsx
@@ -458,9 +458,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -512,6 +509,72 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -547,69 +610,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -937,7 +937,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D4" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -956,521 +956,521 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
     </row>
     <row r="2" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="str">
+      <c r="B2" s="59" t="str">
         <f>"CÔNG TRÌNH: " &amp;"Công trình 1"</f>
         <v>CÔNG TRÌNH: Công trình 1</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
     </row>
     <row r="3" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="38" t="str">
+      <c r="B3" s="59" t="str">
         <f>"HẠNG MỤC: " &amp;"Hạng mục 1"</f>
         <v>HẠNG MỤC: Hạng mục 1</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
-      <c r="U3" s="38"/>
-      <c r="V3" s="38"/>
-      <c r="W3" s="38"/>
-      <c r="X3" s="38"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
     </row>
     <row r="4" spans="1:27" s="7" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="39" t="s">
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="M4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="36" t="s">
+      <c r="N4" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36" t="s">
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36" t="s">
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
+      <c r="W4" s="57"/>
+      <c r="X4" s="57"/>
       <c r="Y4" s="5"/>
     </row>
     <row r="5" spans="1:27" s="7" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="8" t="s">
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="8" t="s">
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="O5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="8" t="s">
+      <c r="Q5" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="8" t="s">
+      <c r="R5" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="8" t="s">
+      <c r="S5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="8" t="s">
+      <c r="T5" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="8" t="s">
+      <c r="U5" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="V5" s="8" t="s">
+      <c r="V5" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="W5" s="8" t="s">
+      <c r="W5" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="X5" s="8" t="s">
+      <c r="X5" s="52" t="s">
         <v>22</v>
       </c>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="50"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="17"/>
+    <row r="6" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="16"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
     </row>
-    <row r="7" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="57"/>
-      <c r="P7" s="57"/>
-      <c r="Q7" s="57"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="17"/>
+    <row r="7" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="16"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
     </row>
-    <row r="8" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="55"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="57"/>
-      <c r="O8" s="57"/>
-      <c r="P8" s="57"/>
-      <c r="Q8" s="57"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="17"/>
+    <row r="8" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="38"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="16"/>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
     </row>
-    <row r="9" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="57"/>
-      <c r="O9" s="57"/>
-      <c r="P9" s="57"/>
-      <c r="Q9" s="57"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="17"/>
+    <row r="9" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="16"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
     </row>
-    <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="57"/>
-      <c r="P10" s="57"/>
-      <c r="Q10" s="57"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="17"/>
+    <row r="10" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="16"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
     </row>
-    <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="57"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="17"/>
+    <row r="11" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="16"/>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="57"/>
-      <c r="P12" s="57"/>
-      <c r="Q12" s="57"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="17"/>
+    <row r="12" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="16"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
     </row>
-    <row r="13" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="55"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="57"/>
-      <c r="P13" s="57"/>
-      <c r="Q13" s="57"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="17"/>
+    <row r="13" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="16"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="57"/>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="17"/>
+    <row r="14" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="44"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="16"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="61"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="63"/>
-      <c r="N15" s="64"/>
-      <c r="O15" s="64"/>
-      <c r="P15" s="64"/>
-      <c r="Q15" s="64"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="16"/>
-      <c r="W15" s="16"/>
-      <c r="X15" s="16"/>
-      <c r="Y15" s="17"/>
+    <row r="15" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="45"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="51"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="16"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+    <row r="16" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="9">
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="8">
         <f>SUMIF(B6:B15,"&gt;0",R6:R15)</f>
         <v>0</v>
       </c>
-      <c r="S16" s="9">
+      <c r="S16" s="8">
         <f>SUMIF(B6:B15,"&gt;0",S6:S15)</f>
         <v>0</v>
       </c>
-      <c r="T16" s="9">
+      <c r="T16" s="8">
         <f>SUMIF(B6:B15,"&gt;0",T6:T15)</f>
         <v>0</v>
       </c>
-      <c r="U16" s="9">
+      <c r="U16" s="8">
         <f>SUMIF(B6:B15,"&gt;0",U6:U15)</f>
         <v>0</v>
       </c>
@@ -1562,312 +1562,312 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="18" t="s">
+      <c r="M4" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="N4" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="O4" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="17" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
     </row>
     <row r="6" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
     </row>
     <row r="7" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
     </row>
     <row r="8" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
     </row>
     <row r="9" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
     </row>
     <row r="10" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
     </row>
     <row r="11" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
     </row>
     <row r="12" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
     </row>
     <row r="13" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
     </row>
     <row r="14" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="24"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="23"/>
     </row>
     <row r="15" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="29"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>